<commit_message>
add evaluation for BIO in model.py
</commit_message>
<xml_diff>
--- a/NLP_Project2/f_measure result.xlsx
+++ b/NLP_Project2/f_measure result.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
   <si>
     <t>single feature</t>
   </si>
@@ -54,13 +54,19 @@
   </si>
   <si>
     <t>multiple features</t>
+  </si>
+  <si>
+    <t>B-CUE</t>
+  </si>
+  <si>
+    <t>I-CUE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -68,16 +74,36 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -85,12 +111,34 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -368,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:N13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -380,83 +428,396 @@
     <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C1" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B2" t="s">
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N2" s="1"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2">
-        <v>0.96434273549799998</v>
-      </c>
-      <c r="D2">
-        <v>0.96578249336900002</v>
-      </c>
-      <c r="E2">
-        <v>0.96839042454699997</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="C3" s="1">
+        <v>0.13</v>
+      </c>
+      <c r="D3" s="2">
+        <v>151</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="F3" s="2">
+        <v>236</v>
+      </c>
+      <c r="G3" s="2">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="H3" s="2">
+        <v>151</v>
+      </c>
+      <c r="I3" s="2">
+        <v>0.21</v>
+      </c>
+      <c r="J3" s="2">
+        <v>236</v>
+      </c>
+      <c r="K3" s="2">
+        <v>0.49</v>
+      </c>
+      <c r="L3" s="2">
+        <v>151</v>
+      </c>
+      <c r="M3" s="2">
+        <v>0.39</v>
+      </c>
+      <c r="N3" s="2">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="6">
+        <f>(C3*D3+E3*F3)/(D3+F3)</f>
+        <v>0.11170542635658916</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="6">
+        <f>(G3*H3+I3*J3)/(H3+J3)</f>
+        <v>0.23731266149870803</v>
+      </c>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="6">
+        <f>(K3*L3+M3*N3)/(L3+N3)</f>
+        <v>0.42901808785529716</v>
+      </c>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="1"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C3">
-        <v>0.98167873881599998</v>
-      </c>
-      <c r="D3">
-        <v>0.98167873881599998</v>
-      </c>
-      <c r="E3">
-        <v>0.221479314668</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B4" t="s">
+      <c r="C5" s="7">
+        <v>0</v>
+      </c>
+      <c r="D5" s="2">
+        <v>151</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0</v>
+      </c>
+      <c r="F5" s="2">
+        <v>236</v>
+      </c>
+      <c r="G5" s="2">
+        <v>0</v>
+      </c>
+      <c r="H5" s="2">
+        <v>151</v>
+      </c>
+      <c r="I5" s="2">
+        <v>0</v>
+      </c>
+      <c r="J5" s="2">
+        <v>236</v>
+      </c>
+      <c r="K5" s="2">
+        <v>0</v>
+      </c>
+      <c r="L5" s="2">
+        <v>151</v>
+      </c>
+      <c r="M5" s="2">
+        <v>0.03</v>
+      </c>
+      <c r="N5" s="2">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="6">
+        <f>(C5*D5+E5*F5)/(D5+F5)</f>
+        <v>0</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="6">
+        <f>(G5*H5+I5*J5)/(H5+J5)</f>
+        <v>0</v>
+      </c>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="6">
+        <f>(K5*L5+M5*N5)/(L5+N5)</f>
+        <v>1.8294573643410854E-2</v>
+      </c>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="1"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C4">
-        <v>0.96354443853100002</v>
-      </c>
-      <c r="D4">
-        <v>0.96587301587300001</v>
-      </c>
-      <c r="E4">
-        <v>0.96720663769299997</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B5" t="s">
+      <c r="C7" s="1">
+        <v>0.11</v>
+      </c>
+      <c r="D7" s="2">
+        <v>151</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0.06</v>
+      </c>
+      <c r="F7" s="2">
+        <v>236</v>
+      </c>
+      <c r="G7" s="2">
+        <v>0.39</v>
+      </c>
+      <c r="H7" s="2">
+        <v>151</v>
+      </c>
+      <c r="I7" s="2">
+        <v>0.33</v>
+      </c>
+      <c r="J7" s="2">
+        <v>236</v>
+      </c>
+      <c r="K7" s="2">
+        <v>0.51</v>
+      </c>
+      <c r="L7" s="2">
+        <v>151</v>
+      </c>
+      <c r="M7" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="N7" s="2">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="6">
+        <f>(C7*D7+E7*F7)/(D7+F7)</f>
+        <v>7.9509043927648584E-2</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="6">
+        <f>(G7*H7+I7*J7)/(H7+J7)</f>
+        <v>0.35341085271317835</v>
+      </c>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="6">
+        <f>(K7*L7+M7*N7)/(L7+N7)</f>
+        <v>0.44291989664082693</v>
+      </c>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="1"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C5">
-        <v>0.96637309847899999</v>
-      </c>
-      <c r="D5">
-        <v>0.96770764119599995</v>
-      </c>
-      <c r="E5">
-        <v>0.96979332273399999</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="C9" s="1">
+        <v>0.06</v>
+      </c>
+      <c r="D9" s="2">
+        <v>151</v>
+      </c>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2">
+        <v>0.24</v>
+      </c>
+      <c r="H9" s="2">
+        <v>151</v>
+      </c>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2">
+        <v>0.42</v>
+      </c>
+      <c r="L9" s="2">
+        <v>151</v>
+      </c>
+      <c r="M9" s="2"/>
+      <c r="N9" s="1"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="6">
+        <f>(C9*D9+E9*F9)/(D9+F9)</f>
+        <v>6.0000000000000005E-2</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="6">
+        <f>(G9*H9+I9*J9)/(H9+J9)</f>
+        <v>0.24000000000000002</v>
+      </c>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="6">
+        <f>(K9*L9+M9*N9)/(L9+N9)</f>
+        <v>0.42</v>
+      </c>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="1"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="3"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D7">
-        <v>0.98</v>
-      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1">
+        <v>0.54</v>
+      </c>
+      <c r="D12" s="2">
+        <v>151</v>
+      </c>
+      <c r="E12" s="2">
+        <v>0.54</v>
+      </c>
+      <c r="F12" s="2">
+        <v>236</v>
+      </c>
+      <c r="G12" s="2">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="H12" s="2">
+        <v>151</v>
+      </c>
+      <c r="I12" s="2">
+        <v>0.52</v>
+      </c>
+      <c r="J12" s="2">
+        <v>236</v>
+      </c>
+      <c r="K12" s="2">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="L12" s="2">
+        <v>151</v>
+      </c>
+      <c r="M12" s="2">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="N12" s="2">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="6">
+        <f>(C12*D12+E12*F12)/(D12+F12)</f>
+        <v>0.54</v>
+      </c>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="6">
+        <f>(G12*H12+I12*J12)/(H12+J12)</f>
+        <v>0.53170542635658913</v>
+      </c>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="6">
+        <f>(K12*L12+M12*N12)/(L12+N12)</f>
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>